<commit_message>
finish the excel uploading part and add the function of viewing excel
</commit_message>
<xml_diff>
--- a/public/upload/upload.xlsx
+++ b/public/upload/upload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>updatetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -487,6 +487,23 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+      <c r="C5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extends the mrjsontable plugins and completed initial screen module
</commit_message>
<xml_diff>
--- a/public/upload/upload.xlsx
+++ b/public/upload/upload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>updatetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -487,23 +487,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>123</v>
-      </c>
-      <c r="C5">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add the saiku library and the graph controller
</commit_message>
<xml_diff>
--- a/public/upload/upload.xlsx
+++ b/public/upload/upload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>updatetime</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -444,7 +444,7 @@
         <v>456</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -478,13 +478,30 @@
         <v>963</v>
       </c>
       <c r="C4">
-        <v>22.3</v>
+        <v>15.9</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+      <c r="C5">
+        <v>22.5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>